<commit_message>
Add Lunne sample quality function
</commit_message>
<xml_diff>
--- a/tests/siteinvestigation/insitutests/data/output_pcpt.xlsx
+++ b/tests/siteinvestigation/insitutests/data/output_pcpt.xlsx
@@ -9625,7 +9625,7 @@
         <v>6.75</v>
       </c>
       <c r="M168" t="n">
-        <v>34.03</v>
+        <v>34.02999999999999</v>
       </c>
       <c r="N168" t="n">
         <v>25.57</v>
@@ -10925,7 +10925,7 @@
         <v>6.75</v>
       </c>
       <c r="M193" t="n">
-        <v>39.155</v>
+        <v>39.15499999999999</v>
       </c>
       <c r="N193" t="n">
         <v>28.945</v>
@@ -11133,7 +11133,7 @@
         <v>6.75</v>
       </c>
       <c r="M197" t="n">
-        <v>39.97499999999999</v>
+        <v>39.975</v>
       </c>
       <c r="N197" t="n">
         <v>29.485</v>
@@ -11448,7 +11448,7 @@
         <v>41.205</v>
       </c>
       <c r="N203" t="n">
-        <v>30.29499999999999</v>
+        <v>30.295</v>
       </c>
       <c r="O203" t="n">
         <v>71.5</v>
@@ -11653,7 +11653,7 @@
         <v>6.75</v>
       </c>
       <c r="M207" t="n">
-        <v>42.02499999999999</v>
+        <v>42.025</v>
       </c>
       <c r="N207" t="n">
         <v>30.835</v>
@@ -12384,7 +12384,7 @@
         <v>44.895</v>
       </c>
       <c r="N221" t="n">
-        <v>32.72499999999999</v>
+        <v>32.725</v>
       </c>
       <c r="O221" t="n">
         <v>77.62</v>
@@ -12543,7 +12543,7 @@
         <v>33.13</v>
       </c>
       <c r="O224" t="n">
-        <v>78.64000000000001</v>
+        <v>78.64</v>
       </c>
       <c r="P224" t="n">
         <v>0.8</v>
@@ -12644,7 +12644,7 @@
         <v>45.92</v>
       </c>
       <c r="N226" t="n">
-        <v>33.40000000000001</v>
+        <v>33.4</v>
       </c>
       <c r="O226" t="n">
         <v>79.32000000000001</v>
@@ -12907,7 +12907,7 @@
         <v>34.075</v>
       </c>
       <c r="O231" t="n">
-        <v>81.02000000000001</v>
+        <v>81.02</v>
       </c>
       <c r="P231" t="n">
         <v>0.8</v>
@@ -12953,13 +12953,13 @@
         <v>6.75</v>
       </c>
       <c r="M232" t="n">
-        <v>47.14999999999999</v>
+        <v>47.15</v>
       </c>
       <c r="N232" t="n">
         <v>34.20999999999999</v>
       </c>
       <c r="O232" t="n">
-        <v>81.35999999999999</v>
+        <v>81.36</v>
       </c>
       <c r="P232" t="n">
         <v>0.8</v>
@@ -13112,7 +13112,7 @@
         <v>47.765</v>
       </c>
       <c r="N235" t="n">
-        <v>34.61499999999999</v>
+        <v>34.615</v>
       </c>
       <c r="O235" t="n">
         <v>82.38</v>
@@ -13164,7 +13164,7 @@
         <v>47.97</v>
       </c>
       <c r="N236" t="n">
-        <v>34.75</v>
+        <v>34.74999999999999</v>
       </c>
       <c r="O236" t="n">
         <v>82.72</v>
@@ -13369,7 +13369,7 @@
         <v>6.75</v>
       </c>
       <c r="M240" t="n">
-        <v>48.78999999999999</v>
+        <v>48.79</v>
       </c>
       <c r="N240" t="n">
         <v>35.29</v>
@@ -13843,7 +13843,7 @@
         <v>36.505</v>
       </c>
       <c r="O249" t="n">
-        <v>87.14000000000001</v>
+        <v>87.14</v>
       </c>
       <c r="P249" t="n">
         <v>0.8</v>
@@ -14207,7 +14207,7 @@
         <v>37.45</v>
       </c>
       <c r="O256" t="n">
-        <v>89.52000000000001</v>
+        <v>89.52</v>
       </c>
       <c r="P256" t="n">
         <v>0.8</v>
@@ -14253,13 +14253,13 @@
         <v>6.75</v>
       </c>
       <c r="M257" t="n">
-        <v>52.27499999999999</v>
+        <v>52.275</v>
       </c>
       <c r="N257" t="n">
         <v>37.58499999999999</v>
       </c>
       <c r="O257" t="n">
-        <v>89.85999999999999</v>
+        <v>89.86</v>
       </c>
       <c r="P257" t="n">
         <v>0.8</v>
@@ -14571,7 +14571,7 @@
         <v>38.395</v>
       </c>
       <c r="O263" t="n">
-        <v>91.90000000000001</v>
+        <v>91.89999999999999</v>
       </c>
       <c r="P263" t="n">
         <v>0.8</v>
@@ -14669,10 +14669,10 @@
         <v>6.75</v>
       </c>
       <c r="M265" t="n">
-        <v>53.91499999999999</v>
+        <v>53.915</v>
       </c>
       <c r="N265" t="n">
-        <v>38.66499999999999</v>
+        <v>38.665</v>
       </c>
       <c r="O265" t="n">
         <v>92.58</v>
@@ -14831,7 +14831,7 @@
         <v>39.07</v>
       </c>
       <c r="O268" t="n">
-        <v>93.59999999999999</v>
+        <v>93.60000000000001</v>
       </c>
       <c r="P268" t="n">
         <v>0.8</v>
@@ -15143,7 +15143,7 @@
         <v>39.88</v>
       </c>
       <c r="O274" t="n">
-        <v>95.64000000000001</v>
+        <v>95.64</v>
       </c>
       <c r="P274" t="n">
         <v>0.8</v>
@@ -15192,10 +15192,10 @@
         <v>55.965</v>
       </c>
       <c r="N275" t="n">
-        <v>40.015</v>
+        <v>40.01499999999999</v>
       </c>
       <c r="O275" t="n">
-        <v>95.97999999999999</v>
+        <v>95.98</v>
       </c>
       <c r="P275" t="n">
         <v>0.8</v>
@@ -15400,7 +15400,7 @@
         <v>56.785</v>
       </c>
       <c r="N279" t="n">
-        <v>40.55499999999999</v>
+        <v>40.555</v>
       </c>
       <c r="O279" t="n">
         <v>97.34</v>
@@ -15452,7 +15452,7 @@
         <v>56.98999999999999</v>
       </c>
       <c r="N280" t="n">
-        <v>40.69</v>
+        <v>40.68999999999999</v>
       </c>
       <c r="O280" t="n">
         <v>97.67999999999999</v>
@@ -15507,7 +15507,7 @@
         <v>40.825</v>
       </c>
       <c r="O281" t="n">
-        <v>98.02000000000001</v>
+        <v>98.02</v>
       </c>
       <c r="P281" t="n">
         <v>0.8</v>
@@ -15553,13 +15553,13 @@
         <v>6.75</v>
       </c>
       <c r="M282" t="n">
-        <v>57.39999999999999</v>
+        <v>57.4</v>
       </c>
       <c r="N282" t="n">
         <v>40.95999999999999</v>
       </c>
       <c r="O282" t="n">
-        <v>98.35999999999999</v>
+        <v>98.36</v>
       </c>
       <c r="P282" t="n">
         <v>0.8</v>
@@ -15660,7 +15660,7 @@
         <v>57.81</v>
       </c>
       <c r="N284" t="n">
-        <v>41.22999999999999</v>
+        <v>41.23</v>
       </c>
       <c r="O284" t="n">
         <v>99.03999999999999</v>
@@ -15969,7 +15969,7 @@
         <v>6.75</v>
       </c>
       <c r="M290" t="n">
-        <v>59.03999999999999</v>
+        <v>59.04</v>
       </c>
       <c r="N290" t="n">
         <v>42.03999999999999</v>
@@ -16128,7 +16128,7 @@
         <v>59.655</v>
       </c>
       <c r="N293" t="n">
-        <v>42.44499999999999</v>
+        <v>42.445</v>
       </c>
       <c r="O293" t="n">
         <v>102.1</v>
@@ -17792,7 +17792,7 @@
         <v>66.215</v>
       </c>
       <c r="N325" t="n">
-        <v>48.16499999999999</v>
+        <v>48.165</v>
       </c>
       <c r="O325" t="n">
         <v>114.38</v>
@@ -18832,7 +18832,7 @@
         <v>70.315</v>
       </c>
       <c r="N345" t="n">
-        <v>51.86499999999999</v>
+        <v>51.865</v>
       </c>
       <c r="O345" t="n">
         <v>122.18</v>
@@ -18985,7 +18985,7 @@
         <v>9.25</v>
       </c>
       <c r="M348" t="n">
-        <v>70.93000000000001</v>
+        <v>70.92999999999999</v>
       </c>
       <c r="N348" t="n">
         <v>52.41999999999999</v>
@@ -19092,7 +19092,7 @@
         <v>71.34</v>
       </c>
       <c r="N350" t="n">
-        <v>52.78999999999999</v>
+        <v>52.79</v>
       </c>
       <c r="O350" t="n">
         <v>124.13</v>
@@ -19401,7 +19401,7 @@
         <v>9.25</v>
       </c>
       <c r="M356" t="n">
-        <v>72.56999999999999</v>
+        <v>72.57000000000001</v>
       </c>
       <c r="N356" t="n">
         <v>53.9</v>
@@ -20132,7 +20132,7 @@
         <v>75.44</v>
       </c>
       <c r="N370" t="n">
-        <v>56.48999999999999</v>
+        <v>56.49</v>
       </c>
       <c r="O370" t="n">
         <v>131.93</v>
@@ -20392,7 +20392,7 @@
         <v>76.465</v>
       </c>
       <c r="N375" t="n">
-        <v>57.41499999999999</v>
+        <v>57.415</v>
       </c>
       <c r="O375" t="n">
         <v>133.88</v>
@@ -20701,7 +20701,7 @@
         <v>9.25</v>
       </c>
       <c r="M381" t="n">
-        <v>77.69499999999999</v>
+        <v>77.69500000000001</v>
       </c>
       <c r="N381" t="n">
         <v>58.525</v>
@@ -20753,7 +20753,7 @@
         <v>9.25</v>
       </c>
       <c r="M382" t="n">
-        <v>77.90000000000001</v>
+        <v>77.89999999999999</v>
       </c>
       <c r="N382" t="n">
         <v>58.70999999999999</v>
@@ -20860,7 +20860,7 @@
         <v>78.31</v>
       </c>
       <c r="N384" t="n">
-        <v>59.08</v>
+        <v>59.07999999999999</v>
       </c>
       <c r="O384" t="n">
         <v>137.39</v>
@@ -20964,7 +20964,7 @@
         <v>78.72</v>
       </c>
       <c r="N386" t="n">
-        <v>59.44999999999999</v>
+        <v>59.45</v>
       </c>
       <c r="O386" t="n">
         <v>138.17</v>
@@ -21013,7 +21013,7 @@
         <v>9.25</v>
       </c>
       <c r="M387" t="n">
-        <v>78.92500000000001</v>
+        <v>78.925</v>
       </c>
       <c r="N387" t="n">
         <v>59.635</v>
@@ -21432,7 +21432,7 @@
         <v>80.565</v>
       </c>
       <c r="N395" t="n">
-        <v>61.11499999999999</v>
+        <v>61.115</v>
       </c>
       <c r="O395" t="n">
         <v>141.68</v>
@@ -21692,7 +21692,7 @@
         <v>81.59</v>
       </c>
       <c r="N400" t="n">
-        <v>62.03999999999999</v>
+        <v>62.04</v>
       </c>
       <c r="O400" t="n">
         <v>143.63</v>
@@ -22053,7 +22053,7 @@
         <v>9.25</v>
       </c>
       <c r="M407" t="n">
-        <v>83.02500000000001</v>
+        <v>83.02499999999999</v>
       </c>
       <c r="N407" t="n">
         <v>63.33499999999999</v>
@@ -22368,7 +22368,7 @@
         <v>84.25500000000001</v>
       </c>
       <c r="N413" t="n">
-        <v>64.44499999999999</v>
+        <v>64.44500000000001</v>
       </c>
       <c r="O413" t="n">
         <v>148.7</v>
@@ -22469,7 +22469,7 @@
         <v>9.25</v>
       </c>
       <c r="M415" t="n">
-        <v>84.66499999999999</v>
+        <v>84.66500000000001</v>
       </c>
       <c r="N415" t="n">
         <v>64.815</v>
@@ -22573,7 +22573,7 @@
         <v>9.25</v>
       </c>
       <c r="M417" t="n">
-        <v>85.07500000000002</v>
+        <v>85.075</v>
       </c>
       <c r="N417" t="n">
         <v>65.185</v>
@@ -22784,7 +22784,7 @@
         <v>85.89500000000001</v>
       </c>
       <c r="N421" t="n">
-        <v>65.92500000000001</v>
+        <v>65.925</v>
       </c>
       <c r="O421" t="n">
         <v>151.82</v>
@@ -22888,7 +22888,7 @@
         <v>86.30500000000001</v>
       </c>
       <c r="N423" t="n">
-        <v>66.29499999999999</v>
+        <v>66.295</v>
       </c>
       <c r="O423" t="n">
         <v>152.6</v>
@@ -22989,7 +22989,7 @@
         <v>9.25</v>
       </c>
       <c r="M425" t="n">
-        <v>86.715</v>
+        <v>86.71500000000002</v>
       </c>
       <c r="N425" t="n">
         <v>66.66500000000001</v>
@@ -23304,7 +23304,7 @@
         <v>87.94500000000001</v>
       </c>
       <c r="N431" t="n">
-        <v>67.77500000000001</v>
+        <v>67.77499999999999</v>
       </c>
       <c r="O431" t="n">
         <v>155.72</v>
@@ -23668,7 +23668,7 @@
         <v>89.38000000000001</v>
       </c>
       <c r="N438" t="n">
-        <v>69.06999999999999</v>
+        <v>69.07000000000001</v>
       </c>
       <c r="O438" t="n">
         <v>158.45</v>
@@ -23769,7 +23769,7 @@
         <v>9.25</v>
       </c>
       <c r="M440" t="n">
-        <v>89.78999999999999</v>
+        <v>89.79000000000001</v>
       </c>
       <c r="N440" t="n">
         <v>69.44</v>
@@ -23821,7 +23821,7 @@
         <v>9.25</v>
       </c>
       <c r="M441" t="n">
-        <v>89.995</v>
+        <v>89.99499999999999</v>
       </c>
       <c r="N441" t="n">
         <v>69.62499999999999</v>
@@ -24084,7 +24084,7 @@
         <v>91.02000000000001</v>
       </c>
       <c r="N446" t="n">
-        <v>70.55000000000001</v>
+        <v>70.55</v>
       </c>
       <c r="O446" t="n">
         <v>161.57</v>
@@ -24188,7 +24188,7 @@
         <v>91.43000000000001</v>
       </c>
       <c r="N448" t="n">
-        <v>70.91999999999999</v>
+        <v>70.92</v>
       </c>
       <c r="O448" t="n">
         <v>162.35</v>
@@ -24237,7 +24237,7 @@
         <v>9.25</v>
       </c>
       <c r="M449" t="n">
-        <v>91.63499999999999</v>
+        <v>91.63500000000001</v>
       </c>
       <c r="N449" t="n">
         <v>71.10499999999999</v>
@@ -24289,7 +24289,7 @@
         <v>9.25</v>
       </c>
       <c r="M450" t="n">
-        <v>91.84</v>
+        <v>91.84000000000002</v>
       </c>
       <c r="N450" t="n">
         <v>71.29000000000001</v>
@@ -24341,7 +24341,7 @@
         <v>9.25</v>
       </c>
       <c r="M451" t="n">
-        <v>92.04500000000002</v>
+        <v>92.045</v>
       </c>
       <c r="N451" t="n">
         <v>71.47499999999999</v>
@@ -24604,7 +24604,7 @@
         <v>93.07000000000001</v>
       </c>
       <c r="N456" t="n">
-        <v>72.40000000000001</v>
+        <v>72.39999999999999</v>
       </c>
       <c r="O456" t="n">
         <v>165.47</v>
@@ -24809,7 +24809,7 @@
         <v>9.25</v>
       </c>
       <c r="M460" t="n">
-        <v>93.89000000000001</v>
+        <v>93.89</v>
       </c>
       <c r="N460" t="n">
         <v>73.14</v>
@@ -24968,7 +24968,7 @@
         <v>94.50500000000001</v>
       </c>
       <c r="N463" t="n">
-        <v>73.69499999999999</v>
+        <v>73.69500000000001</v>
       </c>
       <c r="O463" t="n">
         <v>168.2</v>
@@ -25069,7 +25069,7 @@
         <v>9.25</v>
       </c>
       <c r="M465" t="n">
-        <v>94.91499999999999</v>
+        <v>94.91500000000001</v>
       </c>
       <c r="N465" t="n">
         <v>74.065</v>
@@ -25121,7 +25121,7 @@
         <v>9.25</v>
       </c>
       <c r="M466" t="n">
-        <v>95.12</v>
+        <v>95.11999999999999</v>
       </c>
       <c r="N466" t="n">
         <v>74.24999999999999</v>
@@ -25332,7 +25332,7 @@
         <v>95.94</v>
       </c>
       <c r="N470" t="n">
-        <v>74.98999999999998</v>
+        <v>74.98999999999999</v>
       </c>
       <c r="O470" t="n">
         <v>170.93</v>
@@ -25384,7 +25384,7 @@
         <v>96.14500000000001</v>
       </c>
       <c r="N471" t="n">
-        <v>75.17500000000001</v>
+        <v>75.175</v>
       </c>
       <c r="O471" t="n">
         <v>171.32</v>
@@ -25488,7 +25488,7 @@
         <v>96.55500000000001</v>
       </c>
       <c r="N473" t="n">
-        <v>75.54499999999999</v>
+        <v>75.545</v>
       </c>
       <c r="O473" t="n">
         <v>172.1</v>
@@ -25537,7 +25537,7 @@
         <v>9.25</v>
       </c>
       <c r="M474" t="n">
-        <v>96.75999999999999</v>
+        <v>96.76000000000001</v>
       </c>
       <c r="N474" t="n">
         <v>75.72999999999999</v>
@@ -25589,7 +25589,7 @@
         <v>9.25</v>
       </c>
       <c r="M475" t="n">
-        <v>96.965</v>
+        <v>96.96500000000002</v>
       </c>
       <c r="N475" t="n">
         <v>75.91500000000001</v>
@@ -25641,7 +25641,7 @@
         <v>9.25</v>
       </c>
       <c r="M476" t="n">
-        <v>97.17000000000002</v>
+        <v>97.17</v>
       </c>
       <c r="N476" t="n">
         <v>76.09999999999999</v>
@@ -25904,7 +25904,7 @@
         <v>98.19500000000001</v>
       </c>
       <c r="N481" t="n">
-        <v>77.02500000000001</v>
+        <v>77.02499999999999</v>
       </c>
       <c r="O481" t="n">
         <v>175.22</v>
@@ -26057,7 +26057,7 @@
         <v>9.25</v>
       </c>
       <c r="M484" t="n">
-        <v>98.81</v>
+        <v>98.81000000000002</v>
       </c>
       <c r="N484" t="n">
         <v>77.58</v>
@@ -26109,7 +26109,7 @@
         <v>9.25</v>
       </c>
       <c r="M485" t="n">
-        <v>99.01500000000001</v>
+        <v>99.015</v>
       </c>
       <c r="N485" t="n">
         <v>77.765</v>
@@ -26268,7 +26268,7 @@
         <v>99.63000000000001</v>
       </c>
       <c r="N488" t="n">
-        <v>78.31999999999999</v>
+        <v>78.32000000000001</v>
       </c>
       <c r="O488" t="n">
         <v>177.95</v>
@@ -26424,7 +26424,7 @@
         <v>100.245</v>
       </c>
       <c r="N491" t="n">
-        <v>78.875</v>
+        <v>78.87499999999999</v>
       </c>
       <c r="O491" t="n">
         <v>179.12</v>
@@ -26632,7 +26632,7 @@
         <v>101.065</v>
       </c>
       <c r="N495" t="n">
-        <v>79.61499999999998</v>
+        <v>79.61499999999999</v>
       </c>
       <c r="O495" t="n">
         <v>180.68</v>
@@ -26684,7 +26684,7 @@
         <v>101.27</v>
       </c>
       <c r="N496" t="n">
-        <v>79.80000000000001</v>
+        <v>79.8</v>
       </c>
       <c r="O496" t="n">
         <v>181.07</v>
@@ -26788,7 +26788,7 @@
         <v>101.68</v>
       </c>
       <c r="N498" t="n">
-        <v>80.16999999999999</v>
+        <v>80.17</v>
       </c>
       <c r="O498" t="n">
         <v>181.85</v>
@@ -27204,7 +27204,7 @@
         <v>103.32</v>
       </c>
       <c r="N506" t="n">
-        <v>81.65000000000001</v>
+        <v>81.64999999999999</v>
       </c>
       <c r="O506" t="n">
         <v>184.97</v>
@@ -27568,7 +27568,7 @@
         <v>104.755</v>
       </c>
       <c r="N513" t="n">
-        <v>82.94499999999999</v>
+        <v>82.94500000000001</v>
       </c>
       <c r="O513" t="n">
         <v>187.7</v>
@@ -27724,7 +27724,7 @@
         <v>105.37</v>
       </c>
       <c r="N516" t="n">
-        <v>83.5</v>
+        <v>83.49999999999999</v>
       </c>
       <c r="O516" t="n">
         <v>188.87</v>
@@ -27932,7 +27932,7 @@
         <v>106.19</v>
       </c>
       <c r="N520" t="n">
-        <v>84.23999999999998</v>
+        <v>84.23999999999999</v>
       </c>
       <c r="O520" t="n">
         <v>190.43</v>
@@ -27984,7 +27984,7 @@
         <v>106.395</v>
       </c>
       <c r="N521" t="n">
-        <v>84.42500000000001</v>
+        <v>84.425</v>
       </c>
       <c r="O521" t="n">
         <v>190.82</v>
@@ -28088,7 +28088,7 @@
         <v>106.805</v>
       </c>
       <c r="N523" t="n">
-        <v>84.79499999999999</v>
+        <v>84.795</v>
       </c>
       <c r="O523" t="n">
         <v>191.6</v>
@@ -28504,7 +28504,7 @@
         <v>108.445</v>
       </c>
       <c r="N531" t="n">
-        <v>86.27500000000001</v>
+        <v>86.27499999999999</v>
       </c>
       <c r="O531" t="n">
         <v>194.72</v>
@@ -28868,7 +28868,7 @@
         <v>109.88</v>
       </c>
       <c r="N538" t="n">
-        <v>87.56999999999999</v>
+        <v>87.57000000000001</v>
       </c>
       <c r="O538" t="n">
         <v>197.45</v>
@@ -29024,7 +29024,7 @@
         <v>110.495</v>
       </c>
       <c r="N541" t="n">
-        <v>88.125</v>
+        <v>88.12499999999999</v>
       </c>
       <c r="O541" t="n">
         <v>198.62</v>
@@ -29232,7 +29232,7 @@
         <v>111.315</v>
       </c>
       <c r="N545" t="n">
-        <v>88.86499999999998</v>
+        <v>88.86499999999999</v>
       </c>
       <c r="O545" t="n">
         <v>200.18</v>
@@ -29284,7 +29284,7 @@
         <v>111.52</v>
       </c>
       <c r="N546" t="n">
-        <v>89.05000000000001</v>
+        <v>89.05</v>
       </c>
       <c r="O546" t="n">
         <v>200.57</v>
@@ -29388,7 +29388,7 @@
         <v>111.93</v>
       </c>
       <c r="N548" t="n">
-        <v>89.41999999999999</v>
+        <v>89.42</v>
       </c>
       <c r="O548" t="n">
         <v>201.35</v>
@@ -29804,7 +29804,7 @@
         <v>113.57</v>
       </c>
       <c r="N556" t="n">
-        <v>90.90000000000001</v>
+        <v>90.89999999999999</v>
       </c>
       <c r="O556" t="n">
         <v>204.47</v>
@@ -30168,7 +30168,7 @@
         <v>115.005</v>
       </c>
       <c r="N563" t="n">
-        <v>92.19499999999999</v>
+        <v>92.19500000000001</v>
       </c>
       <c r="O563" t="n">
         <v>207.2</v>
@@ -30324,7 +30324,7 @@
         <v>115.62</v>
       </c>
       <c r="N566" t="n">
-        <v>92.75</v>
+        <v>92.74999999999999</v>
       </c>
       <c r="O566" t="n">
         <v>208.37</v>
@@ -30532,10 +30532,10 @@
         <v>116.44</v>
       </c>
       <c r="N570" t="n">
-        <v>93.48999999999998</v>
+        <v>93.48999999999999</v>
       </c>
       <c r="O570" t="n">
-        <v>209.9299999999999</v>
+        <v>209.93</v>
       </c>
       <c r="P570" t="n">
         <v>0.8</v>
@@ -30584,7 +30584,7 @@
         <v>116.645</v>
       </c>
       <c r="N571" t="n">
-        <v>93.67500000000001</v>
+        <v>93.675</v>
       </c>
       <c r="O571" t="n">
         <v>210.32</v>
@@ -30688,7 +30688,7 @@
         <v>117.055</v>
       </c>
       <c r="N573" t="n">
-        <v>94.04499999999999</v>
+        <v>94.045</v>
       </c>
       <c r="O573" t="n">
         <v>211.1</v>
@@ -31104,7 +31104,7 @@
         <v>118.695</v>
       </c>
       <c r="N581" t="n">
-        <v>95.52500000000001</v>
+        <v>95.52499999999999</v>
       </c>
       <c r="O581" t="n">
         <v>214.22</v>
@@ -31419,7 +31419,7 @@
         <v>96.63499999999999</v>
       </c>
       <c r="O587" t="n">
-        <v>216.5599999999999</v>
+        <v>216.56</v>
       </c>
       <c r="P587" t="n">
         <v>0.8</v>
@@ -31468,7 +31468,7 @@
         <v>120.13</v>
       </c>
       <c r="N588" t="n">
-        <v>96.81999999999999</v>
+        <v>96.82000000000001</v>
       </c>
       <c r="O588" t="n">
         <v>216.95</v>
@@ -31624,10 +31624,10 @@
         <v>120.745</v>
       </c>
       <c r="N591" t="n">
-        <v>97.375</v>
+        <v>97.37499999999999</v>
       </c>
       <c r="O591" t="n">
-        <v>218.1199999999999</v>
+        <v>218.12</v>
       </c>
       <c r="P591" t="n">
         <v>0.8</v>
@@ -31832,10 +31832,10 @@
         <v>121.565</v>
       </c>
       <c r="N595" t="n">
-        <v>98.11499999999998</v>
+        <v>98.11499999999999</v>
       </c>
       <c r="O595" t="n">
-        <v>219.6799999999999</v>
+        <v>219.68</v>
       </c>
       <c r="P595" t="n">
         <v>0.8</v>
@@ -31884,7 +31884,7 @@
         <v>121.77</v>
       </c>
       <c r="N596" t="n">
-        <v>98.30000000000001</v>
+        <v>98.3</v>
       </c>
       <c r="O596" t="n">
         <v>220.07</v>
@@ -31988,7 +31988,7 @@
         <v>122.18</v>
       </c>
       <c r="N598" t="n">
-        <v>98.66999999999999</v>
+        <v>98.67</v>
       </c>
       <c r="O598" t="n">
         <v>220.85</v>
@@ -32511,7 +32511,7 @@
         <v>100.52</v>
       </c>
       <c r="O608" t="n">
-        <v>224.7499999999999</v>
+        <v>224.75</v>
       </c>
       <c r="P608" t="n">
         <v>0.8</v>
@@ -32719,7 +32719,7 @@
         <v>101.26</v>
       </c>
       <c r="O612" t="n">
-        <v>226.3099999999999</v>
+        <v>226.31</v>
       </c>
       <c r="P612" t="n">
         <v>0.8</v>
@@ -32927,7 +32927,7 @@
         <v>102</v>
       </c>
       <c r="O616" t="n">
-        <v>227.8699999999999</v>
+        <v>227.87</v>
       </c>
       <c r="P616" t="n">
         <v>0.8</v>
@@ -33135,7 +33135,7 @@
         <v>102.74</v>
       </c>
       <c r="O620" t="n">
-        <v>229.4299999999999</v>
+        <v>229.43</v>
       </c>
       <c r="P620" t="n">
         <v>0.8</v>
@@ -40727,7 +40727,7 @@
         <v>129.96</v>
       </c>
       <c r="O766" t="n">
-        <v>286.5799999999999</v>
+        <v>286.58</v>
       </c>
       <c r="P766" t="n">
         <v>0.8</v>
@@ -41715,7 +41715,7 @@
         <v>133.665</v>
       </c>
       <c r="O785" t="n">
-        <v>294.1799999999999</v>
+        <v>294.18</v>
       </c>
       <c r="P785" t="n">
         <v>0.8</v>
@@ -50139,7 +50139,7 @@
         <v>165.255</v>
       </c>
       <c r="O947" t="n">
-        <v>358.9799999999999</v>
+        <v>358.98</v>
       </c>
       <c r="P947" t="n">
         <v>0.8</v>
@@ -50295,7 +50295,7 @@
         <v>165.84</v>
       </c>
       <c r="O950" t="n">
-        <v>360.1799999999999</v>
+        <v>360.18</v>
       </c>
       <c r="P950" t="n">
         <v>0.8</v>
@@ -50867,7 +50867,7 @@
         <v>167.985</v>
       </c>
       <c r="O961" t="n">
-        <v>364.5799999999999</v>
+        <v>364.58</v>
       </c>
       <c r="P961" t="n">
         <v>0.8</v>
@@ -51439,7 +51439,7 @@
         <v>170.13</v>
       </c>
       <c r="O972" t="n">
-        <v>368.9799999999999</v>
+        <v>368.98</v>
       </c>
       <c r="P972" t="n">
         <v>0.8</v>
@@ -51595,7 +51595,7 @@
         <v>170.715</v>
       </c>
       <c r="O975" t="n">
-        <v>370.1799999999999</v>
+        <v>370.18</v>
       </c>
       <c r="P975" t="n">
         <v>0.8</v>
@@ -52167,7 +52167,7 @@
         <v>172.86</v>
       </c>
       <c r="O986" t="n">
-        <v>374.5799999999999</v>
+        <v>374.58</v>
       </c>
       <c r="P986" t="n">
         <v>0.8</v>
@@ -52531,7 +52531,7 @@
         <v>174.225</v>
       </c>
       <c r="O993" t="n">
-        <v>377.38</v>
+        <v>377.3799999999999</v>
       </c>
       <c r="P993" t="n">
         <v>0.8</v>

</xml_diff>

<commit_message>
Chin-kondler method, group effect and doc fixes
</commit_message>
<xml_diff>
--- a/tests/siteinvestigation/insitutests/data/output_pcpt.xlsx
+++ b/tests/siteinvestigation/insitutests/data/output_pcpt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Location data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cone properties" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Layering" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Location data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cone properties" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Layering" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -9625,7 +9625,7 @@
         <v>6.75</v>
       </c>
       <c r="M168" t="n">
-        <v>34.03</v>
+        <v>34.02999999999999</v>
       </c>
       <c r="N168" t="n">
         <v>25.57</v>
@@ -10925,7 +10925,7 @@
         <v>6.75</v>
       </c>
       <c r="M193" t="n">
-        <v>39.155</v>
+        <v>39.15499999999999</v>
       </c>
       <c r="N193" t="n">
         <v>28.945</v>
@@ -11133,7 +11133,7 @@
         <v>6.75</v>
       </c>
       <c r="M197" t="n">
-        <v>39.97499999999999</v>
+        <v>39.975</v>
       </c>
       <c r="N197" t="n">
         <v>29.485</v>
@@ -11448,7 +11448,7 @@
         <v>41.205</v>
       </c>
       <c r="N203" t="n">
-        <v>30.29499999999999</v>
+        <v>30.295</v>
       </c>
       <c r="O203" t="n">
         <v>71.5</v>
@@ -11653,7 +11653,7 @@
         <v>6.75</v>
       </c>
       <c r="M207" t="n">
-        <v>42.02499999999999</v>
+        <v>42.025</v>
       </c>
       <c r="N207" t="n">
         <v>30.835</v>
@@ -12384,7 +12384,7 @@
         <v>44.895</v>
       </c>
       <c r="N221" t="n">
-        <v>32.72499999999999</v>
+        <v>32.725</v>
       </c>
       <c r="O221" t="n">
         <v>77.62</v>
@@ -12543,7 +12543,7 @@
         <v>33.13</v>
       </c>
       <c r="O224" t="n">
-        <v>78.64000000000001</v>
+        <v>78.64</v>
       </c>
       <c r="P224" t="n">
         <v>0.8</v>
@@ -12644,7 +12644,7 @@
         <v>45.92</v>
       </c>
       <c r="N226" t="n">
-        <v>33.40000000000001</v>
+        <v>33.4</v>
       </c>
       <c r="O226" t="n">
         <v>79.32000000000001</v>
@@ -12907,7 +12907,7 @@
         <v>34.075</v>
       </c>
       <c r="O231" t="n">
-        <v>81.02000000000001</v>
+        <v>81.02</v>
       </c>
       <c r="P231" t="n">
         <v>0.8</v>
@@ -12953,13 +12953,13 @@
         <v>6.75</v>
       </c>
       <c r="M232" t="n">
-        <v>47.14999999999999</v>
+        <v>47.15</v>
       </c>
       <c r="N232" t="n">
         <v>34.20999999999999</v>
       </c>
       <c r="O232" t="n">
-        <v>81.35999999999999</v>
+        <v>81.36</v>
       </c>
       <c r="P232" t="n">
         <v>0.8</v>
@@ -13112,7 +13112,7 @@
         <v>47.765</v>
       </c>
       <c r="N235" t="n">
-        <v>34.61499999999999</v>
+        <v>34.615</v>
       </c>
       <c r="O235" t="n">
         <v>82.38</v>
@@ -13164,7 +13164,7 @@
         <v>47.97</v>
       </c>
       <c r="N236" t="n">
-        <v>34.75</v>
+        <v>34.74999999999999</v>
       </c>
       <c r="O236" t="n">
         <v>82.72</v>
@@ -13369,7 +13369,7 @@
         <v>6.75</v>
       </c>
       <c r="M240" t="n">
-        <v>48.78999999999999</v>
+        <v>48.79</v>
       </c>
       <c r="N240" t="n">
         <v>35.29</v>
@@ -13843,7 +13843,7 @@
         <v>36.505</v>
       </c>
       <c r="O249" t="n">
-        <v>87.14000000000001</v>
+        <v>87.14</v>
       </c>
       <c r="P249" t="n">
         <v>0.8</v>
@@ -14207,7 +14207,7 @@
         <v>37.45</v>
       </c>
       <c r="O256" t="n">
-        <v>89.52000000000001</v>
+        <v>89.52</v>
       </c>
       <c r="P256" t="n">
         <v>0.8</v>
@@ -14253,13 +14253,13 @@
         <v>6.75</v>
       </c>
       <c r="M257" t="n">
-        <v>52.27499999999999</v>
+        <v>52.275</v>
       </c>
       <c r="N257" t="n">
         <v>37.58499999999999</v>
       </c>
       <c r="O257" t="n">
-        <v>89.85999999999999</v>
+        <v>89.86</v>
       </c>
       <c r="P257" t="n">
         <v>0.8</v>
@@ -14571,7 +14571,7 @@
         <v>38.395</v>
       </c>
       <c r="O263" t="n">
-        <v>91.90000000000001</v>
+        <v>91.89999999999999</v>
       </c>
       <c r="P263" t="n">
         <v>0.8</v>
@@ -14669,10 +14669,10 @@
         <v>6.75</v>
       </c>
       <c r="M265" t="n">
-        <v>53.91499999999999</v>
+        <v>53.915</v>
       </c>
       <c r="N265" t="n">
-        <v>38.66499999999999</v>
+        <v>38.665</v>
       </c>
       <c r="O265" t="n">
         <v>92.58</v>
@@ -14831,7 +14831,7 @@
         <v>39.07</v>
       </c>
       <c r="O268" t="n">
-        <v>93.59999999999999</v>
+        <v>93.60000000000001</v>
       </c>
       <c r="P268" t="n">
         <v>0.8</v>
@@ -15143,7 +15143,7 @@
         <v>39.88</v>
       </c>
       <c r="O274" t="n">
-        <v>95.64000000000001</v>
+        <v>95.64</v>
       </c>
       <c r="P274" t="n">
         <v>0.8</v>
@@ -15192,10 +15192,10 @@
         <v>55.965</v>
       </c>
       <c r="N275" t="n">
-        <v>40.015</v>
+        <v>40.01499999999999</v>
       </c>
       <c r="O275" t="n">
-        <v>95.97999999999999</v>
+        <v>95.98</v>
       </c>
       <c r="P275" t="n">
         <v>0.8</v>
@@ -15400,7 +15400,7 @@
         <v>56.785</v>
       </c>
       <c r="N279" t="n">
-        <v>40.55499999999999</v>
+        <v>40.555</v>
       </c>
       <c r="O279" t="n">
         <v>97.34</v>
@@ -15452,7 +15452,7 @@
         <v>56.98999999999999</v>
       </c>
       <c r="N280" t="n">
-        <v>40.69</v>
+        <v>40.68999999999999</v>
       </c>
       <c r="O280" t="n">
         <v>97.67999999999999</v>
@@ -15507,7 +15507,7 @@
         <v>40.825</v>
       </c>
       <c r="O281" t="n">
-        <v>98.02000000000001</v>
+        <v>98.02</v>
       </c>
       <c r="P281" t="n">
         <v>0.8</v>
@@ -15553,13 +15553,13 @@
         <v>6.75</v>
       </c>
       <c r="M282" t="n">
-        <v>57.39999999999999</v>
+        <v>57.4</v>
       </c>
       <c r="N282" t="n">
         <v>40.95999999999999</v>
       </c>
       <c r="O282" t="n">
-        <v>98.35999999999999</v>
+        <v>98.36</v>
       </c>
       <c r="P282" t="n">
         <v>0.8</v>
@@ -15660,7 +15660,7 @@
         <v>57.81</v>
       </c>
       <c r="N284" t="n">
-        <v>41.22999999999999</v>
+        <v>41.23</v>
       </c>
       <c r="O284" t="n">
         <v>99.03999999999999</v>
@@ -15969,7 +15969,7 @@
         <v>6.75</v>
       </c>
       <c r="M290" t="n">
-        <v>59.03999999999999</v>
+        <v>59.04</v>
       </c>
       <c r="N290" t="n">
         <v>42.03999999999999</v>
@@ -16128,7 +16128,7 @@
         <v>59.655</v>
       </c>
       <c r="N293" t="n">
-        <v>42.44499999999999</v>
+        <v>42.445</v>
       </c>
       <c r="O293" t="n">
         <v>102.1</v>
@@ -17792,7 +17792,7 @@
         <v>66.215</v>
       </c>
       <c r="N325" t="n">
-        <v>48.16499999999999</v>
+        <v>48.165</v>
       </c>
       <c r="O325" t="n">
         <v>114.38</v>
@@ -18832,7 +18832,7 @@
         <v>70.315</v>
       </c>
       <c r="N345" t="n">
-        <v>51.86499999999999</v>
+        <v>51.865</v>
       </c>
       <c r="O345" t="n">
         <v>122.18</v>
@@ -18985,7 +18985,7 @@
         <v>9.25</v>
       </c>
       <c r="M348" t="n">
-        <v>70.93000000000001</v>
+        <v>70.92999999999999</v>
       </c>
       <c r="N348" t="n">
         <v>52.41999999999999</v>
@@ -19092,7 +19092,7 @@
         <v>71.34</v>
       </c>
       <c r="N350" t="n">
-        <v>52.78999999999999</v>
+        <v>52.79</v>
       </c>
       <c r="O350" t="n">
         <v>124.13</v>
@@ -19401,7 +19401,7 @@
         <v>9.25</v>
       </c>
       <c r="M356" t="n">
-        <v>72.56999999999999</v>
+        <v>72.57000000000001</v>
       </c>
       <c r="N356" t="n">
         <v>53.9</v>
@@ -20132,7 +20132,7 @@
         <v>75.44</v>
       </c>
       <c r="N370" t="n">
-        <v>56.48999999999999</v>
+        <v>56.49</v>
       </c>
       <c r="O370" t="n">
         <v>131.93</v>
@@ -20392,7 +20392,7 @@
         <v>76.465</v>
       </c>
       <c r="N375" t="n">
-        <v>57.41499999999999</v>
+        <v>57.415</v>
       </c>
       <c r="O375" t="n">
         <v>133.88</v>
@@ -20701,7 +20701,7 @@
         <v>9.25</v>
       </c>
       <c r="M381" t="n">
-        <v>77.69499999999999</v>
+        <v>77.69500000000001</v>
       </c>
       <c r="N381" t="n">
         <v>58.525</v>
@@ -20753,7 +20753,7 @@
         <v>9.25</v>
       </c>
       <c r="M382" t="n">
-        <v>77.90000000000001</v>
+        <v>77.89999999999999</v>
       </c>
       <c r="N382" t="n">
         <v>58.70999999999999</v>
@@ -20860,7 +20860,7 @@
         <v>78.31</v>
       </c>
       <c r="N384" t="n">
-        <v>59.08</v>
+        <v>59.07999999999999</v>
       </c>
       <c r="O384" t="n">
         <v>137.39</v>
@@ -20964,7 +20964,7 @@
         <v>78.72</v>
       </c>
       <c r="N386" t="n">
-        <v>59.44999999999999</v>
+        <v>59.45</v>
       </c>
       <c r="O386" t="n">
         <v>138.17</v>
@@ -21013,7 +21013,7 @@
         <v>9.25</v>
       </c>
       <c r="M387" t="n">
-        <v>78.92500000000001</v>
+        <v>78.925</v>
       </c>
       <c r="N387" t="n">
         <v>59.635</v>
@@ -21432,7 +21432,7 @@
         <v>80.565</v>
       </c>
       <c r="N395" t="n">
-        <v>61.11499999999999</v>
+        <v>61.115</v>
       </c>
       <c r="O395" t="n">
         <v>141.68</v>
@@ -21692,7 +21692,7 @@
         <v>81.59</v>
       </c>
       <c r="N400" t="n">
-        <v>62.03999999999999</v>
+        <v>62.04</v>
       </c>
       <c r="O400" t="n">
         <v>143.63</v>
@@ -22053,7 +22053,7 @@
         <v>9.25</v>
       </c>
       <c r="M407" t="n">
-        <v>83.02500000000001</v>
+        <v>83.02499999999999</v>
       </c>
       <c r="N407" t="n">
         <v>63.33499999999999</v>
@@ -22368,7 +22368,7 @@
         <v>84.25500000000001</v>
       </c>
       <c r="N413" t="n">
-        <v>64.44499999999999</v>
+        <v>64.44500000000001</v>
       </c>
       <c r="O413" t="n">
         <v>148.7</v>
@@ -22469,7 +22469,7 @@
         <v>9.25</v>
       </c>
       <c r="M415" t="n">
-        <v>84.66499999999999</v>
+        <v>84.66500000000001</v>
       </c>
       <c r="N415" t="n">
         <v>64.815</v>
@@ -22573,7 +22573,7 @@
         <v>9.25</v>
       </c>
       <c r="M417" t="n">
-        <v>85.07500000000002</v>
+        <v>85.075</v>
       </c>
       <c r="N417" t="n">
         <v>65.185</v>
@@ -22784,7 +22784,7 @@
         <v>85.89500000000001</v>
       </c>
       <c r="N421" t="n">
-        <v>65.92500000000001</v>
+        <v>65.925</v>
       </c>
       <c r="O421" t="n">
         <v>151.82</v>
@@ -22888,7 +22888,7 @@
         <v>86.30500000000001</v>
       </c>
       <c r="N423" t="n">
-        <v>66.29499999999999</v>
+        <v>66.295</v>
       </c>
       <c r="O423" t="n">
         <v>152.6</v>
@@ -22989,7 +22989,7 @@
         <v>9.25</v>
       </c>
       <c r="M425" t="n">
-        <v>86.715</v>
+        <v>86.71500000000002</v>
       </c>
       <c r="N425" t="n">
         <v>66.66500000000001</v>
@@ -23304,7 +23304,7 @@
         <v>87.94500000000001</v>
       </c>
       <c r="N431" t="n">
-        <v>67.77500000000001</v>
+        <v>67.77499999999999</v>
       </c>
       <c r="O431" t="n">
         <v>155.72</v>
@@ -23668,7 +23668,7 @@
         <v>89.38000000000001</v>
       </c>
       <c r="N438" t="n">
-        <v>69.06999999999999</v>
+        <v>69.07000000000001</v>
       </c>
       <c r="O438" t="n">
         <v>158.45</v>
@@ -23769,7 +23769,7 @@
         <v>9.25</v>
       </c>
       <c r="M440" t="n">
-        <v>89.78999999999999</v>
+        <v>89.79000000000001</v>
       </c>
       <c r="N440" t="n">
         <v>69.44</v>
@@ -23821,7 +23821,7 @@
         <v>9.25</v>
       </c>
       <c r="M441" t="n">
-        <v>89.995</v>
+        <v>89.99499999999999</v>
       </c>
       <c r="N441" t="n">
         <v>69.62499999999999</v>
@@ -24084,7 +24084,7 @@
         <v>91.02000000000001</v>
       </c>
       <c r="N446" t="n">
-        <v>70.55000000000001</v>
+        <v>70.55</v>
       </c>
       <c r="O446" t="n">
         <v>161.57</v>
@@ -24188,7 +24188,7 @@
         <v>91.43000000000001</v>
       </c>
       <c r="N448" t="n">
-        <v>70.91999999999999</v>
+        <v>70.92</v>
       </c>
       <c r="O448" t="n">
         <v>162.35</v>
@@ -24237,7 +24237,7 @@
         <v>9.25</v>
       </c>
       <c r="M449" t="n">
-        <v>91.63499999999999</v>
+        <v>91.63500000000001</v>
       </c>
       <c r="N449" t="n">
         <v>71.10499999999999</v>
@@ -24289,7 +24289,7 @@
         <v>9.25</v>
       </c>
       <c r="M450" t="n">
-        <v>91.84</v>
+        <v>91.84000000000002</v>
       </c>
       <c r="N450" t="n">
         <v>71.29000000000001</v>
@@ -24341,7 +24341,7 @@
         <v>9.25</v>
       </c>
       <c r="M451" t="n">
-        <v>92.04500000000002</v>
+        <v>92.045</v>
       </c>
       <c r="N451" t="n">
         <v>71.47499999999999</v>
@@ -24604,7 +24604,7 @@
         <v>93.07000000000001</v>
       </c>
       <c r="N456" t="n">
-        <v>72.40000000000001</v>
+        <v>72.39999999999999</v>
       </c>
       <c r="O456" t="n">
         <v>165.47</v>
@@ -24809,7 +24809,7 @@
         <v>9.25</v>
       </c>
       <c r="M460" t="n">
-        <v>93.89000000000001</v>
+        <v>93.89</v>
       </c>
       <c r="N460" t="n">
         <v>73.14</v>
@@ -24968,7 +24968,7 @@
         <v>94.50500000000001</v>
       </c>
       <c r="N463" t="n">
-        <v>73.69499999999999</v>
+        <v>73.69500000000001</v>
       </c>
       <c r="O463" t="n">
         <v>168.2</v>
@@ -25069,7 +25069,7 @@
         <v>9.25</v>
       </c>
       <c r="M465" t="n">
-        <v>94.91499999999999</v>
+        <v>94.91500000000001</v>
       </c>
       <c r="N465" t="n">
         <v>74.065</v>
@@ -25121,7 +25121,7 @@
         <v>9.25</v>
       </c>
       <c r="M466" t="n">
-        <v>95.12</v>
+        <v>95.11999999999999</v>
       </c>
       <c r="N466" t="n">
         <v>74.24999999999999</v>
@@ -25332,7 +25332,7 @@
         <v>95.94</v>
       </c>
       <c r="N470" t="n">
-        <v>74.98999999999998</v>
+        <v>74.98999999999999</v>
       </c>
       <c r="O470" t="n">
         <v>170.93</v>
@@ -25384,7 +25384,7 @@
         <v>96.14500000000001</v>
       </c>
       <c r="N471" t="n">
-        <v>75.17500000000001</v>
+        <v>75.175</v>
       </c>
       <c r="O471" t="n">
         <v>171.32</v>
@@ -25488,7 +25488,7 @@
         <v>96.55500000000001</v>
       </c>
       <c r="N473" t="n">
-        <v>75.54499999999999</v>
+        <v>75.545</v>
       </c>
       <c r="O473" t="n">
         <v>172.1</v>
@@ -25537,7 +25537,7 @@
         <v>9.25</v>
       </c>
       <c r="M474" t="n">
-        <v>96.75999999999999</v>
+        <v>96.76000000000001</v>
       </c>
       <c r="N474" t="n">
         <v>75.72999999999999</v>
@@ -25589,7 +25589,7 @@
         <v>9.25</v>
       </c>
       <c r="M475" t="n">
-        <v>96.965</v>
+        <v>96.96500000000002</v>
       </c>
       <c r="N475" t="n">
         <v>75.91500000000001</v>
@@ -25641,7 +25641,7 @@
         <v>9.25</v>
       </c>
       <c r="M476" t="n">
-        <v>97.17000000000002</v>
+        <v>97.17</v>
       </c>
       <c r="N476" t="n">
         <v>76.09999999999999</v>
@@ -25904,7 +25904,7 @@
         <v>98.19500000000001</v>
       </c>
       <c r="N481" t="n">
-        <v>77.02500000000001</v>
+        <v>77.02499999999999</v>
       </c>
       <c r="O481" t="n">
         <v>175.22</v>
@@ -26057,7 +26057,7 @@
         <v>9.25</v>
       </c>
       <c r="M484" t="n">
-        <v>98.81</v>
+        <v>98.81000000000002</v>
       </c>
       <c r="N484" t="n">
         <v>77.58</v>
@@ -26109,7 +26109,7 @@
         <v>9.25</v>
       </c>
       <c r="M485" t="n">
-        <v>99.01500000000001</v>
+        <v>99.015</v>
       </c>
       <c r="N485" t="n">
         <v>77.765</v>
@@ -26268,7 +26268,7 @@
         <v>99.63000000000001</v>
       </c>
       <c r="N488" t="n">
-        <v>78.31999999999999</v>
+        <v>78.32000000000001</v>
       </c>
       <c r="O488" t="n">
         <v>177.95</v>
@@ -26424,7 +26424,7 @@
         <v>100.245</v>
       </c>
       <c r="N491" t="n">
-        <v>78.875</v>
+        <v>78.87499999999999</v>
       </c>
       <c r="O491" t="n">
         <v>179.12</v>
@@ -26632,7 +26632,7 @@
         <v>101.065</v>
       </c>
       <c r="N495" t="n">
-        <v>79.61499999999998</v>
+        <v>79.61499999999999</v>
       </c>
       <c r="O495" t="n">
         <v>180.68</v>
@@ -26684,7 +26684,7 @@
         <v>101.27</v>
       </c>
       <c r="N496" t="n">
-        <v>79.80000000000001</v>
+        <v>79.8</v>
       </c>
       <c r="O496" t="n">
         <v>181.07</v>
@@ -26788,7 +26788,7 @@
         <v>101.68</v>
       </c>
       <c r="N498" t="n">
-        <v>80.16999999999999</v>
+        <v>80.17</v>
       </c>
       <c r="O498" t="n">
         <v>181.85</v>
@@ -27204,7 +27204,7 @@
         <v>103.32</v>
       </c>
       <c r="N506" t="n">
-        <v>81.65000000000001</v>
+        <v>81.64999999999999</v>
       </c>
       <c r="O506" t="n">
         <v>184.97</v>
@@ -27568,7 +27568,7 @@
         <v>104.755</v>
       </c>
       <c r="N513" t="n">
-        <v>82.94499999999999</v>
+        <v>82.94500000000001</v>
       </c>
       <c r="O513" t="n">
         <v>187.7</v>
@@ -27724,7 +27724,7 @@
         <v>105.37</v>
       </c>
       <c r="N516" t="n">
-        <v>83.5</v>
+        <v>83.49999999999999</v>
       </c>
       <c r="O516" t="n">
         <v>188.87</v>
@@ -27932,7 +27932,7 @@
         <v>106.19</v>
       </c>
       <c r="N520" t="n">
-        <v>84.23999999999998</v>
+        <v>84.23999999999999</v>
       </c>
       <c r="O520" t="n">
         <v>190.43</v>
@@ -27984,7 +27984,7 @@
         <v>106.395</v>
       </c>
       <c r="N521" t="n">
-        <v>84.42500000000001</v>
+        <v>84.425</v>
       </c>
       <c r="O521" t="n">
         <v>190.82</v>
@@ -28088,7 +28088,7 @@
         <v>106.805</v>
       </c>
       <c r="N523" t="n">
-        <v>84.79499999999999</v>
+        <v>84.795</v>
       </c>
       <c r="O523" t="n">
         <v>191.6</v>
@@ -28504,7 +28504,7 @@
         <v>108.445</v>
       </c>
       <c r="N531" t="n">
-        <v>86.27500000000001</v>
+        <v>86.27499999999999</v>
       </c>
       <c r="O531" t="n">
         <v>194.72</v>
@@ -28868,7 +28868,7 @@
         <v>109.88</v>
       </c>
       <c r="N538" t="n">
-        <v>87.56999999999999</v>
+        <v>87.57000000000001</v>
       </c>
       <c r="O538" t="n">
         <v>197.45</v>
@@ -29024,7 +29024,7 @@
         <v>110.495</v>
       </c>
       <c r="N541" t="n">
-        <v>88.125</v>
+        <v>88.12499999999999</v>
       </c>
       <c r="O541" t="n">
         <v>198.62</v>
@@ -29232,7 +29232,7 @@
         <v>111.315</v>
       </c>
       <c r="N545" t="n">
-        <v>88.86499999999998</v>
+        <v>88.86499999999999</v>
       </c>
       <c r="O545" t="n">
         <v>200.18</v>
@@ -29284,7 +29284,7 @@
         <v>111.52</v>
       </c>
       <c r="N546" t="n">
-        <v>89.05000000000001</v>
+        <v>89.05</v>
       </c>
       <c r="O546" t="n">
         <v>200.57</v>
@@ -29388,7 +29388,7 @@
         <v>111.93</v>
       </c>
       <c r="N548" t="n">
-        <v>89.41999999999999</v>
+        <v>89.42</v>
       </c>
       <c r="O548" t="n">
         <v>201.35</v>
@@ -29804,7 +29804,7 @@
         <v>113.57</v>
       </c>
       <c r="N556" t="n">
-        <v>90.90000000000001</v>
+        <v>90.89999999999999</v>
       </c>
       <c r="O556" t="n">
         <v>204.47</v>
@@ -30168,7 +30168,7 @@
         <v>115.005</v>
       </c>
       <c r="N563" t="n">
-        <v>92.19499999999999</v>
+        <v>92.19500000000001</v>
       </c>
       <c r="O563" t="n">
         <v>207.2</v>
@@ -30324,7 +30324,7 @@
         <v>115.62</v>
       </c>
       <c r="N566" t="n">
-        <v>92.75</v>
+        <v>92.74999999999999</v>
       </c>
       <c r="O566" t="n">
         <v>208.37</v>
@@ -30532,10 +30532,10 @@
         <v>116.44</v>
       </c>
       <c r="N570" t="n">
-        <v>93.48999999999998</v>
+        <v>93.48999999999999</v>
       </c>
       <c r="O570" t="n">
-        <v>209.9299999999999</v>
+        <v>209.93</v>
       </c>
       <c r="P570" t="n">
         <v>0.8</v>
@@ -30584,7 +30584,7 @@
         <v>116.645</v>
       </c>
       <c r="N571" t="n">
-        <v>93.67500000000001</v>
+        <v>93.675</v>
       </c>
       <c r="O571" t="n">
         <v>210.32</v>
@@ -30688,7 +30688,7 @@
         <v>117.055</v>
       </c>
       <c r="N573" t="n">
-        <v>94.04499999999999</v>
+        <v>94.045</v>
       </c>
       <c r="O573" t="n">
         <v>211.1</v>
@@ -31104,7 +31104,7 @@
         <v>118.695</v>
       </c>
       <c r="N581" t="n">
-        <v>95.52500000000001</v>
+        <v>95.52499999999999</v>
       </c>
       <c r="O581" t="n">
         <v>214.22</v>
@@ -31419,7 +31419,7 @@
         <v>96.63499999999999</v>
       </c>
       <c r="O587" t="n">
-        <v>216.5599999999999</v>
+        <v>216.56</v>
       </c>
       <c r="P587" t="n">
         <v>0.8</v>
@@ -31468,7 +31468,7 @@
         <v>120.13</v>
       </c>
       <c r="N588" t="n">
-        <v>96.81999999999999</v>
+        <v>96.82000000000001</v>
       </c>
       <c r="O588" t="n">
         <v>216.95</v>
@@ -31624,10 +31624,10 @@
         <v>120.745</v>
       </c>
       <c r="N591" t="n">
-        <v>97.375</v>
+        <v>97.37499999999999</v>
       </c>
       <c r="O591" t="n">
-        <v>218.1199999999999</v>
+        <v>218.12</v>
       </c>
       <c r="P591" t="n">
         <v>0.8</v>
@@ -31832,10 +31832,10 @@
         <v>121.565</v>
       </c>
       <c r="N595" t="n">
-        <v>98.11499999999998</v>
+        <v>98.11499999999999</v>
       </c>
       <c r="O595" t="n">
-        <v>219.6799999999999</v>
+        <v>219.68</v>
       </c>
       <c r="P595" t="n">
         <v>0.8</v>
@@ -31884,7 +31884,7 @@
         <v>121.77</v>
       </c>
       <c r="N596" t="n">
-        <v>98.30000000000001</v>
+        <v>98.3</v>
       </c>
       <c r="O596" t="n">
         <v>220.07</v>
@@ -31988,7 +31988,7 @@
         <v>122.18</v>
       </c>
       <c r="N598" t="n">
-        <v>98.66999999999999</v>
+        <v>98.67</v>
       </c>
       <c r="O598" t="n">
         <v>220.85</v>
@@ -32511,7 +32511,7 @@
         <v>100.52</v>
       </c>
       <c r="O608" t="n">
-        <v>224.7499999999999</v>
+        <v>224.75</v>
       </c>
       <c r="P608" t="n">
         <v>0.8</v>
@@ -32719,7 +32719,7 @@
         <v>101.26</v>
       </c>
       <c r="O612" t="n">
-        <v>226.3099999999999</v>
+        <v>226.31</v>
       </c>
       <c r="P612" t="n">
         <v>0.8</v>
@@ -32927,7 +32927,7 @@
         <v>102</v>
       </c>
       <c r="O616" t="n">
-        <v>227.8699999999999</v>
+        <v>227.87</v>
       </c>
       <c r="P616" t="n">
         <v>0.8</v>
@@ -33135,7 +33135,7 @@
         <v>102.74</v>
       </c>
       <c r="O620" t="n">
-        <v>229.4299999999999</v>
+        <v>229.43</v>
       </c>
       <c r="P620" t="n">
         <v>0.8</v>
@@ -40727,7 +40727,7 @@
         <v>129.96</v>
       </c>
       <c r="O766" t="n">
-        <v>286.5799999999999</v>
+        <v>286.58</v>
       </c>
       <c r="P766" t="n">
         <v>0.8</v>
@@ -41715,7 +41715,7 @@
         <v>133.665</v>
       </c>
       <c r="O785" t="n">
-        <v>294.1799999999999</v>
+        <v>294.18</v>
       </c>
       <c r="P785" t="n">
         <v>0.8</v>
@@ -50139,7 +50139,7 @@
         <v>165.255</v>
       </c>
       <c r="O947" t="n">
-        <v>358.9799999999999</v>
+        <v>358.98</v>
       </c>
       <c r="P947" t="n">
         <v>0.8</v>
@@ -50295,7 +50295,7 @@
         <v>165.84</v>
       </c>
       <c r="O950" t="n">
-        <v>360.1799999999999</v>
+        <v>360.18</v>
       </c>
       <c r="P950" t="n">
         <v>0.8</v>
@@ -50867,7 +50867,7 @@
         <v>167.985</v>
       </c>
       <c r="O961" t="n">
-        <v>364.5799999999999</v>
+        <v>364.58</v>
       </c>
       <c r="P961" t="n">
         <v>0.8</v>
@@ -51439,7 +51439,7 @@
         <v>170.13</v>
       </c>
       <c r="O972" t="n">
-        <v>368.9799999999999</v>
+        <v>368.98</v>
       </c>
       <c r="P972" t="n">
         <v>0.8</v>
@@ -51595,7 +51595,7 @@
         <v>170.715</v>
       </c>
       <c r="O975" t="n">
-        <v>370.1799999999999</v>
+        <v>370.18</v>
       </c>
       <c r="P975" t="n">
         <v>0.8</v>
@@ -52167,7 +52167,7 @@
         <v>172.86</v>
       </c>
       <c r="O986" t="n">
-        <v>374.5799999999999</v>
+        <v>374.58</v>
       </c>
       <c r="P986" t="n">
         <v>0.8</v>
@@ -52531,7 +52531,7 @@
         <v>174.225</v>
       </c>
       <c r="O993" t="n">
-        <v>377.38</v>
+        <v>377.3799999999999</v>
       </c>
       <c r="P993" t="n">
         <v>0.8</v>

</xml_diff>